<commit_message>
Convert latitude and longitude to numbers
</commit_message>
<xml_diff>
--- a/results/rentking.xlsx
+++ b/results/rentking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="116">
   <si>
     <t>store_name</t>
   </si>
@@ -43,136 +43,151 @@
     <t>store_hours</t>
   </si>
   <si>
+    <t>Brandon Rent King</t>
+  </si>
+  <si>
+    <t>Bradenton Rent King</t>
+  </si>
+  <si>
     <t>Avon Park Rent King</t>
   </si>
   <si>
+    <t>Pinellas Park Rent King</t>
+  </si>
+  <si>
+    <t>Wauchula Rent King</t>
+  </si>
+  <si>
     <t>Temple Terrace Rent King</t>
   </si>
   <si>
-    <t>Wauchula Rent King</t>
+    <t>Winter Haven Rent King</t>
+  </si>
+  <si>
+    <t>Town N Country Rent King</t>
   </si>
   <si>
     <t>Ruskin Rent King</t>
   </si>
   <si>
-    <t>Town N Country Rent King</t>
+    <t>Haines City Rent King</t>
   </si>
   <si>
     <t>New Port Richey Rent King</t>
   </si>
   <si>
-    <t>Winter Haven Rent King</t>
+    <t>Lake Wales Rent King</t>
   </si>
   <si>
     <t>North Tampa Rent King</t>
   </si>
   <si>
-    <t>Pinellas Park Rent King</t>
+    <t>Riverview Rent King</t>
   </si>
   <si>
     <t>Largo Rent King</t>
   </si>
   <si>
+    <t>Clair Mel Rent King</t>
+  </si>
+  <si>
     <t>Lakeland Rent King</t>
   </si>
   <si>
-    <t>Lake Wales Rent King</t>
-  </si>
-  <si>
-    <t>Haines City Rent King</t>
-  </si>
-  <si>
-    <t>Clair Mel Rent King</t>
-  </si>
-  <si>
-    <t>Riverview Rent King</t>
-  </si>
-  <si>
-    <t>Brandon Rent King</t>
-  </si>
-  <si>
-    <t>Bradenton Rent King</t>
-  </si>
-  <si>
     <t>Central Tampa / Ybor Rent King</t>
   </si>
   <si>
+    <t>609 W. Brandon Blvd.</t>
+  </si>
+  <si>
+    <t>4615 14th St W</t>
+  </si>
+  <si>
     <t>810 US 27 S</t>
   </si>
   <si>
+    <t>6384 66th Street N.</t>
+  </si>
+  <si>
+    <t>1109 U.S. Hwy 17 South</t>
+  </si>
+  <si>
     <t>8727 Temple Terrace Highway</t>
   </si>
   <si>
-    <t>1109 U.S. Hwy 17 South</t>
+    <t>2808 Recker Hwy</t>
+  </si>
+  <si>
+    <t>7523 W. Hillsborough Ave.</t>
   </si>
   <si>
     <t>615 US Hwy 41 South</t>
   </si>
   <si>
-    <t>7523 W. Hillsborough Ave.</t>
+    <t>500 E. Hinson Avenue</t>
   </si>
   <si>
     <t>6107 SR 54</t>
   </si>
   <si>
-    <t>2808 Recker Hwy</t>
+    <t>1960 SR 60 East</t>
   </si>
   <si>
     <t>2267 E. Bearss Ave.</t>
   </si>
   <si>
-    <t>6384 66th Street N.</t>
+    <t>10431 Gibsonton Drive</t>
   </si>
   <si>
     <t>11902 Seminole Blvd.</t>
   </si>
   <si>
+    <t>7466 Palm River Road</t>
+  </si>
+  <si>
     <t>2610 US Hwy 92 East</t>
   </si>
   <si>
-    <t>1960 SR 60 East</t>
-  </si>
-  <si>
-    <t>500 E. Hinson Avenue</t>
-  </si>
-  <si>
-    <t>7466 Palm River Road</t>
-  </si>
-  <si>
-    <t>10431 Gibsonton Drive</t>
-  </si>
-  <si>
-    <t>609 W. Brandon Blvd.</t>
-  </si>
-  <si>
-    <t>4615 14th St W</t>
-  </si>
-  <si>
     <t>2726 Nebraska Ave.</t>
   </si>
   <si>
+    <t>Brandon</t>
+  </si>
+  <si>
+    <t>Bradenton</t>
+  </si>
+  <si>
     <t>Avon Park</t>
   </si>
   <si>
+    <t>Pinellas Park</t>
+  </si>
+  <si>
+    <t>Wauchula</t>
+  </si>
+  <si>
     <t>Temple Terrace</t>
   </si>
   <si>
-    <t>Wauchula</t>
+    <t>Winter Haven</t>
+  </si>
+  <si>
+    <t>Tampa</t>
   </si>
   <si>
     <t>Ruskin</t>
   </si>
   <si>
-    <t>Tampa</t>
+    <t>Haines City</t>
   </si>
   <si>
     <t>New Port Richey</t>
   </si>
   <si>
-    <t>Winter Haven</t>
-  </si>
-  <si>
-    <t>Pinellas Park</t>
+    <t>Lake Wales</t>
+  </si>
+  <si>
+    <t>Riverview</t>
   </si>
   <si>
     <t>Largo</t>
@@ -181,235 +196,166 @@
     <t>Lakeland</t>
   </si>
   <si>
-    <t>Lake Wales</t>
-  </si>
-  <si>
-    <t>Haines City</t>
-  </si>
-  <si>
-    <t>Riverview</t>
-  </si>
-  <si>
-    <t>Brandon</t>
-  </si>
-  <si>
-    <t>Bradenton</t>
-  </si>
-  <si>
     <t>FL</t>
   </si>
   <si>
+    <t>33511</t>
+  </si>
+  <si>
+    <t>34207</t>
+  </si>
+  <si>
     <t>33825</t>
   </si>
   <si>
+    <t>33781</t>
+  </si>
+  <si>
+    <t>33873</t>
+  </si>
+  <si>
     <t>33637</t>
   </si>
   <si>
-    <t>33873</t>
+    <t>33880</t>
+  </si>
+  <si>
+    <t>33615</t>
   </si>
   <si>
     <t>33570</t>
   </si>
   <si>
-    <t>33615</t>
+    <t>33844</t>
   </si>
   <si>
     <t>34653</t>
   </si>
   <si>
-    <t>33880</t>
+    <t>33853</t>
   </si>
   <si>
     <t>33613</t>
   </si>
   <si>
-    <t>33781</t>
+    <t>33569</t>
   </si>
   <si>
     <t>33778</t>
   </si>
   <si>
+    <t>33619</t>
+  </si>
+  <si>
     <t>33801</t>
   </si>
   <si>
-    <t>33853</t>
-  </si>
-  <si>
-    <t>33844</t>
-  </si>
-  <si>
-    <t>33619</t>
-  </si>
-  <si>
-    <t>33569</t>
-  </si>
-  <si>
-    <t>33511</t>
-  </si>
-  <si>
-    <t>34207</t>
-  </si>
-  <si>
     <t>33602</t>
   </si>
   <si>
-    <t>27.58789</t>
-  </si>
-  <si>
-    <t>28.030867</t>
-  </si>
-  <si>
-    <t>27.561504</t>
-  </si>
-  <si>
-    <t>27.71359</t>
-  </si>
-  <si>
-    <t>27.998325</t>
-  </si>
-  <si>
-    <t>28.218555</t>
-  </si>
-  <si>
-    <t>28.019163</t>
-  </si>
-  <si>
-    <t>28.081621</t>
-  </si>
-  <si>
-    <t>27.829819</t>
-  </si>
-  <si>
-    <t>27.8804</t>
-  </si>
-  <si>
-    <t>28.049204</t>
-  </si>
-  <si>
-    <t>27.892109</t>
-  </si>
-  <si>
-    <t>28.106955</t>
-  </si>
-  <si>
-    <t>27.942356</t>
-  </si>
-  <si>
-    <t>27.856718</t>
-  </si>
-  <si>
-    <t>27.936647</t>
-  </si>
-  <si>
-    <t>27.457602</t>
-  </si>
-  <si>
-    <t>27.96715</t>
+    <t>-82.29305</t>
+  </si>
+  <si>
+    <t>-82.57471</t>
   </si>
   <si>
     <t>-81.51457</t>
   </si>
   <si>
+    <t>-82.72896</t>
+  </si>
+  <si>
+    <t>-81.81487</t>
+  </si>
+  <si>
     <t>-82.3559</t>
   </si>
   <si>
-    <t>-81.81487</t>
+    <t>-81.76476</t>
+  </si>
+  <si>
+    <t>-82.56354</t>
   </si>
   <si>
     <t>-82.4345</t>
   </si>
   <si>
-    <t>-82.56354</t>
+    <t>-81.627014</t>
   </si>
   <si>
     <t>-82.713776</t>
   </si>
   <si>
-    <t>-81.76476</t>
+    <t>-81.5578</t>
   </si>
   <si>
     <t>-82.4329</t>
   </si>
   <si>
-    <t>-82.72896</t>
+    <t>-82.33165</t>
   </si>
   <si>
     <t>-82.78874</t>
   </si>
   <si>
+    <t>-82.37178</t>
+  </si>
+  <si>
     <t>-81.90769</t>
   </si>
   <si>
-    <t>-81.5578</t>
-  </si>
-  <si>
-    <t>-81.627014</t>
-  </si>
-  <si>
-    <t>-82.37178</t>
-  </si>
-  <si>
-    <t>-82.33165</t>
-  </si>
-  <si>
-    <t>-82.29305</t>
-  </si>
-  <si>
-    <t>-82.57471</t>
-  </si>
-  <si>
     <t>-82.451485</t>
   </si>
   <si>
+    <t>813-685-6400</t>
+  </si>
+  <si>
+    <t>941-758-9559</t>
+  </si>
+  <si>
     <t>863-453-2400</t>
   </si>
   <si>
+    <t>727-548-6700</t>
+  </si>
+  <si>
+    <t>863-773-4009</t>
+  </si>
+  <si>
     <t>813-988-5115</t>
   </si>
   <si>
-    <t>863-773-4009</t>
+    <t>863-294-8180</t>
+  </si>
+  <si>
+    <t>813-889-9710</t>
   </si>
   <si>
     <t>813-649-1960</t>
   </si>
   <si>
-    <t>813-889-9710</t>
+    <t>863-419-1111</t>
   </si>
   <si>
     <t>727-846-7400</t>
   </si>
   <si>
-    <t>863-294-8180</t>
+    <t>863-678-1929</t>
   </si>
   <si>
     <t>813-910-4200</t>
   </si>
   <si>
-    <t>727-548-6700</t>
+    <t>813-672-1988</t>
   </si>
   <si>
     <t>727-559-0559</t>
   </si>
   <si>
+    <t>813-630-9399</t>
+  </si>
+  <si>
     <t>863-802-1928</t>
-  </si>
-  <si>
-    <t>863-678-1929</t>
-  </si>
-  <si>
-    <t>863-419-1111</t>
-  </si>
-  <si>
-    <t>813-630-9399</t>
-  </si>
-  <si>
-    <t>813-672-1988</t>
-  </si>
-  <si>
-    <t>813-685-6400</t>
-  </si>
-  <si>
-    <t>941-758-9559</t>
   </si>
   <si>
     <t>813-223-9109</t>
@@ -827,17 +773,17 @@
       <c r="E2" t="s">
         <v>61</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2">
+        <v>27.936647</v>
+      </c>
+      <c r="G2" t="s">
         <v>79</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>97</v>
       </c>
-      <c r="H2" t="s">
-        <v>115</v>
-      </c>
       <c r="I2" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -856,17 +802,17 @@
       <c r="E3" t="s">
         <v>62</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3">
+        <v>27.457602</v>
+      </c>
+      <c r="G3" t="s">
         <v>80</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>98</v>
       </c>
-      <c r="H3" t="s">
-        <v>116</v>
-      </c>
       <c r="I3" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -885,17 +831,17 @@
       <c r="E4" t="s">
         <v>63</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4">
+        <v>27.58789</v>
+      </c>
+      <c r="G4" t="s">
         <v>81</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>99</v>
       </c>
-      <c r="H4" t="s">
-        <v>117</v>
-      </c>
       <c r="I4" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -914,17 +860,17 @@
       <c r="E5" t="s">
         <v>64</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5">
+        <v>27.829819</v>
+      </c>
+      <c r="G5" t="s">
         <v>82</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>100</v>
       </c>
-      <c r="H5" t="s">
-        <v>118</v>
-      </c>
       <c r="I5" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -943,17 +889,17 @@
       <c r="E6" t="s">
         <v>65</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6">
+        <v>27.561504</v>
+      </c>
+      <c r="G6" t="s">
         <v>83</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>101</v>
       </c>
-      <c r="H6" t="s">
-        <v>119</v>
-      </c>
       <c r="I6" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -972,17 +918,17 @@
       <c r="E7" t="s">
         <v>66</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7">
+        <v>28.030867</v>
+      </c>
+      <c r="G7" t="s">
         <v>84</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>102</v>
       </c>
-      <c r="H7" t="s">
-        <v>120</v>
-      </c>
       <c r="I7" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1001,17 +947,17 @@
       <c r="E8" t="s">
         <v>67</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8">
+        <v>28.019163</v>
+      </c>
+      <c r="G8" t="s">
         <v>85</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>103</v>
       </c>
-      <c r="H8" t="s">
-        <v>121</v>
-      </c>
       <c r="I8" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1022,7 +968,7 @@
         <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
         <v>60</v>
@@ -1030,17 +976,17 @@
       <c r="E9" t="s">
         <v>68</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9">
+        <v>27.998325</v>
+      </c>
+      <c r="G9" t="s">
         <v>86</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>104</v>
       </c>
-      <c r="H9" t="s">
-        <v>122</v>
-      </c>
       <c r="I9" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1051,7 +997,7 @@
         <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
         <v>60</v>
@@ -1059,17 +1005,17 @@
       <c r="E10" t="s">
         <v>69</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10">
+        <v>27.71359</v>
+      </c>
+      <c r="G10" t="s">
         <v>87</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>105</v>
       </c>
-      <c r="H10" t="s">
-        <v>123</v>
-      </c>
       <c r="I10" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1080,7 +1026,7 @@
         <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
         <v>60</v>
@@ -1088,17 +1034,17 @@
       <c r="E11" t="s">
         <v>70</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11">
+        <v>28.106955</v>
+      </c>
+      <c r="G11" t="s">
         <v>88</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>106</v>
       </c>
-      <c r="H11" t="s">
-        <v>124</v>
-      </c>
       <c r="I11" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1109,7 +1055,7 @@
         <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
         <v>60</v>
@@ -1117,17 +1063,17 @@
       <c r="E12" t="s">
         <v>71</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12">
+        <v>28.218555</v>
+      </c>
+      <c r="G12" t="s">
         <v>89</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>107</v>
       </c>
-      <c r="H12" t="s">
-        <v>125</v>
-      </c>
       <c r="I12" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1138,7 +1084,7 @@
         <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
         <v>60</v>
@@ -1146,17 +1092,17 @@
       <c r="E13" t="s">
         <v>72</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13">
+        <v>27.892109</v>
+      </c>
+      <c r="G13" t="s">
         <v>90</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>108</v>
       </c>
-      <c r="H13" t="s">
-        <v>126</v>
-      </c>
       <c r="I13" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1167,7 +1113,7 @@
         <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
         <v>60</v>
@@ -1175,17 +1121,17 @@
       <c r="E14" t="s">
         <v>73</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14">
+        <v>28.081621</v>
+      </c>
+      <c r="G14" t="s">
         <v>91</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>109</v>
       </c>
-      <c r="H14" t="s">
-        <v>127</v>
-      </c>
       <c r="I14" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1196,7 +1142,7 @@
         <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
         <v>60</v>
@@ -1204,17 +1150,17 @@
       <c r="E15" t="s">
         <v>74</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15">
+        <v>27.856718</v>
+      </c>
+      <c r="G15" t="s">
         <v>92</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>110</v>
       </c>
-      <c r="H15" t="s">
-        <v>128</v>
-      </c>
       <c r="I15" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1225,7 +1171,7 @@
         <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
         <v>60</v>
@@ -1233,17 +1179,17 @@
       <c r="E16" t="s">
         <v>75</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16">
+        <v>27.8804</v>
+      </c>
+      <c r="G16" t="s">
         <v>93</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>111</v>
       </c>
-      <c r="H16" t="s">
-        <v>129</v>
-      </c>
       <c r="I16" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1254,7 +1200,7 @@
         <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
         <v>60</v>
@@ -1262,17 +1208,17 @@
       <c r="E17" t="s">
         <v>76</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17">
+        <v>27.942356</v>
+      </c>
+      <c r="G17" t="s">
         <v>94</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>112</v>
       </c>
-      <c r="H17" t="s">
-        <v>130</v>
-      </c>
       <c r="I17" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1291,17 +1237,17 @@
       <c r="E18" t="s">
         <v>77</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18">
+        <v>28.049204</v>
+      </c>
+      <c r="G18" t="s">
         <v>95</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>113</v>
       </c>
-      <c r="H18" t="s">
-        <v>131</v>
-      </c>
       <c r="I18" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1312,7 +1258,7 @@
         <v>44</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D19" t="s">
         <v>60</v>
@@ -1320,17 +1266,17 @@
       <c r="E19" t="s">
         <v>78</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19">
+        <v>27.96715</v>
+      </c>
+      <c r="G19" t="s">
         <v>96</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>114</v>
       </c>
-      <c r="H19" t="s">
-        <v>132</v>
-      </c>
       <c r="I19" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>